<commit_message>
Update de notas pre examen
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
+++ b/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1194,8 +1194,8 @@
   <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1374,12 +1374,15 @@
       <c r="H5">
         <v>17</v>
       </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1490,12 +1493,15 @@
       <c r="H10">
         <v>18</v>
       </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,12 +1546,15 @@
       <c r="H12">
         <v>18</v>
       </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1565,12 +1574,15 @@
       <c r="H13">
         <v>18</v>
       </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1612,12 +1624,15 @@
       <c r="H15">
         <v>18</v>
       </c>
+      <c r="J15">
+        <v>20</v>
+      </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1703,12 +1718,15 @@
       <c r="H19">
         <v>18</v>
       </c>
+      <c r="J19">
+        <v>20</v>
+      </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1728,12 +1746,15 @@
       <c r="H20">
         <v>18</v>
       </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1753,12 +1774,15 @@
       <c r="H21">
         <v>18</v>
       </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="N21">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,12 +2103,15 @@
       <c r="H35">
         <v>18</v>
       </c>
+      <c r="J35">
+        <v>20</v>
+      </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2129,12 +2156,15 @@
       <c r="H37">
         <v>14</v>
       </c>
+      <c r="J37">
+        <v>20</v>
+      </c>
       <c r="K37">
         <v>1</v>
       </c>
       <c r="N37">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2251,12 +2281,15 @@
       <c r="H42">
         <v>18</v>
       </c>
+      <c r="J42">
+        <v>20</v>
+      </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="N42">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2276,12 +2309,15 @@
       <c r="H43">
         <v>18</v>
       </c>
+      <c r="J43">
+        <v>20</v>
+      </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="N43">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2301,12 +2337,15 @@
       <c r="H44">
         <v>18</v>
       </c>
+      <c r="J44">
+        <v>20</v>
+      </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="N44">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2958,12 +2997,15 @@
       <c r="H71">
         <v>23</v>
       </c>
+      <c r="J71">
+        <v>20</v>
+      </c>
       <c r="K71">
         <v>1</v>
       </c>
       <c r="N71">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2983,12 +3025,15 @@
       <c r="H72">
         <v>23</v>
       </c>
+      <c r="J72">
+        <v>20</v>
+      </c>
       <c r="K72">
         <v>1</v>
       </c>
       <c r="N72">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3033,12 +3078,15 @@
       <c r="H74">
         <v>18</v>
       </c>
+      <c r="J74">
+        <v>20</v>
+      </c>
       <c r="K74">
         <v>1</v>
       </c>
       <c r="N74">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,12 +3306,15 @@
       <c r="H83">
         <v>23</v>
       </c>
+      <c r="J83">
+        <v>20</v>
+      </c>
       <c r="K83">
         <v>1</v>
       </c>
       <c r="N83">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3283,12 +3334,15 @@
       <c r="H84">
         <v>23</v>
       </c>
+      <c r="J84">
+        <v>20</v>
+      </c>
       <c r="K84">
         <v>1</v>
       </c>
       <c r="N84">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3358,12 +3412,15 @@
       <c r="H87">
         <v>23</v>
       </c>
+      <c r="J87">
+        <v>20</v>
+      </c>
       <c r="K87">
         <v>1</v>
       </c>
       <c r="N87">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Notas Examenes de base de datos
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
+++ b/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$93</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -652,7 +652,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1194,8 +1194,8 @@
   <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1399,12 +1399,15 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6"/>
+      <c r="J6">
+        <v>12</v>
+      </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1468,12 +1471,15 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="6"/>
+      <c r="J9">
+        <v>12</v>
+      </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1521,12 +1527,15 @@
       <c r="H11">
         <v>16</v>
       </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1599,12 +1608,18 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6"/>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1671,12 +1686,15 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="6"/>
+      <c r="J17">
+        <v>12</v>
+      </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1909,12 +1927,18 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="6"/>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="J27">
+        <v>14</v>
+      </c>
       <c r="K27">
         <v>1</v>
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1931,12 +1955,15 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="6"/>
+      <c r="H28">
+        <v>15</v>
+      </c>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1956,12 +1983,15 @@
       <c r="H29">
         <v>15</v>
       </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1981,12 +2011,15 @@
       <c r="H30">
         <v>15</v>
       </c>
+      <c r="J30">
+        <v>12</v>
+      </c>
       <c r="K30">
         <v>1</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2006,12 +2039,15 @@
       <c r="H31">
         <v>17</v>
       </c>
+      <c r="J31">
+        <v>12</v>
+      </c>
       <c r="K31">
         <v>1</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2028,12 +2064,18 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="6"/>
+      <c r="H32">
+        <v>15</v>
+      </c>
+      <c r="J32">
+        <v>14</v>
+      </c>
       <c r="K32">
         <v>1</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2053,12 +2095,15 @@
       <c r="H33">
         <v>15</v>
       </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
       <c r="K33">
         <v>1</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,12 +2254,15 @@
       <c r="H39">
         <v>17</v>
       </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
       <c r="K39">
         <v>1</v>
       </c>
       <c r="N39">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2256,12 +2304,15 @@
       <c r="H41">
         <v>14</v>
       </c>
+      <c r="J41">
+        <v>16</v>
+      </c>
       <c r="K41">
         <v>1</v>
       </c>
       <c r="N41">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,12 +2416,15 @@
       <c r="H45">
         <v>17</v>
       </c>
+      <c r="J45">
+        <v>8</v>
+      </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="N45">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2390,12 +2444,15 @@
       <c r="H46">
         <v>17</v>
       </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
       <c r="K46">
         <v>1</v>
       </c>
       <c r="N46">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2440,12 +2497,15 @@
       <c r="H48">
         <v>17</v>
       </c>
+      <c r="J48">
+        <v>14</v>
+      </c>
       <c r="K48">
         <v>1</v>
       </c>
       <c r="N48">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2487,12 +2547,15 @@
       <c r="H50">
         <v>17</v>
       </c>
+      <c r="J50">
+        <v>14</v>
+      </c>
       <c r="K50">
         <v>1</v>
       </c>
       <c r="N50">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2512,12 +2575,15 @@
       <c r="H51">
         <v>14</v>
       </c>
+      <c r="J51">
+        <v>14</v>
+      </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="N51">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2537,12 +2603,15 @@
       <c r="H52">
         <v>15</v>
       </c>
+      <c r="J52">
+        <v>6</v>
+      </c>
       <c r="K52">
         <v>1</v>
       </c>
       <c r="N52">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2584,12 +2653,15 @@
       <c r="H54">
         <v>14</v>
       </c>
+      <c r="J54">
+        <v>14</v>
+      </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="N54">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2606,12 +2678,18 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="6"/>
+      <c r="H55">
+        <v>15</v>
+      </c>
+      <c r="J55">
+        <v>12</v>
+      </c>
       <c r="K55">
         <v>1</v>
       </c>
       <c r="N55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2631,12 +2709,15 @@
       <c r="H56">
         <v>17</v>
       </c>
+      <c r="J56">
+        <v>10</v>
+      </c>
       <c r="K56">
         <v>1</v>
       </c>
       <c r="N56">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2675,12 +2756,18 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="6"/>
+      <c r="H58">
+        <v>15</v>
+      </c>
+      <c r="J58">
+        <v>12</v>
+      </c>
       <c r="K58">
         <v>1</v>
       </c>
       <c r="N58">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2750,12 +2837,15 @@
       <c r="H61">
         <v>15</v>
       </c>
+      <c r="I61">
+        <v>16</v>
+      </c>
       <c r="K61">
         <v>1</v>
       </c>
       <c r="N61">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2775,12 +2865,15 @@
       <c r="H62">
         <v>14</v>
       </c>
+      <c r="J62">
+        <v>12</v>
+      </c>
       <c r="K62">
         <v>1</v>
       </c>
       <c r="N62">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2800,12 +2893,15 @@
       <c r="H63">
         <v>14</v>
       </c>
+      <c r="J63">
+        <v>12</v>
+      </c>
       <c r="K63">
         <v>1</v>
       </c>
       <c r="N63">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2825,12 +2921,15 @@
       <c r="H64">
         <v>14</v>
       </c>
+      <c r="J64">
+        <v>10</v>
+      </c>
       <c r="K64">
         <v>1</v>
       </c>
       <c r="N64">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2850,12 +2949,15 @@
       <c r="H65">
         <v>17</v>
       </c>
+      <c r="J65">
+        <v>12</v>
+      </c>
       <c r="K65">
         <v>1</v>
       </c>
       <c r="N65">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2897,12 +2999,15 @@
       <c r="H67">
         <v>17</v>
       </c>
+      <c r="J67">
+        <v>12</v>
+      </c>
       <c r="K67">
         <v>1</v>
       </c>
       <c r="N67">
         <f t="shared" ref="N67:N99" si="1">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,12 +3052,15 @@
       <c r="H69">
         <v>17</v>
       </c>
+      <c r="J69">
+        <v>8</v>
+      </c>
       <c r="K69">
         <v>1</v>
       </c>
       <c r="N69">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2972,12 +3080,15 @@
       <c r="H70">
         <v>16</v>
       </c>
+      <c r="J70">
+        <v>12</v>
+      </c>
       <c r="K70">
         <v>1</v>
       </c>
       <c r="N70">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,12 +3164,15 @@
       <c r="H73">
         <v>14</v>
       </c>
+      <c r="J73">
+        <v>16</v>
+      </c>
       <c r="K73">
         <v>1</v>
       </c>
       <c r="N73">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3106,12 +3220,15 @@
       <c r="H75">
         <v>14</v>
       </c>
+      <c r="J75">
+        <v>14</v>
+      </c>
       <c r="K75">
         <v>1</v>
       </c>
       <c r="N75">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3131,12 +3248,15 @@
       <c r="H76">
         <v>14</v>
       </c>
+      <c r="J76">
+        <v>10</v>
+      </c>
       <c r="K76">
         <v>1</v>
       </c>
       <c r="N76">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3156,12 +3276,15 @@
       <c r="H77">
         <v>14</v>
       </c>
+      <c r="J77">
+        <v>12</v>
+      </c>
       <c r="K77">
         <v>1</v>
       </c>
       <c r="N77">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3181,12 +3304,15 @@
       <c r="H78">
         <v>14</v>
       </c>
+      <c r="J78">
+        <v>12</v>
+      </c>
       <c r="K78">
         <v>1</v>
       </c>
       <c r="N78">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3231,12 +3357,15 @@
       <c r="H80">
         <v>16</v>
       </c>
+      <c r="J80">
+        <v>12</v>
+      </c>
       <c r="K80">
         <v>1</v>
       </c>
       <c r="N80">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3281,12 +3410,15 @@
       <c r="H82">
         <v>14</v>
       </c>
+      <c r="J82">
+        <v>10</v>
+      </c>
       <c r="K82">
         <v>1</v>
       </c>
       <c r="N82">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3362,12 +3494,15 @@
       <c r="H85">
         <v>17</v>
       </c>
+      <c r="J85">
+        <v>16</v>
+      </c>
       <c r="K85">
         <v>1</v>
       </c>
       <c r="N85">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3387,12 +3522,15 @@
       <c r="H86">
         <v>14</v>
       </c>
+      <c r="J86">
+        <v>16</v>
+      </c>
       <c r="K86">
         <v>1</v>
       </c>
       <c r="N86">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3440,12 +3578,15 @@
       <c r="H88">
         <v>14</v>
       </c>
+      <c r="J88">
+        <v>14</v>
+      </c>
       <c r="K88">
         <v>1</v>
       </c>
       <c r="N88">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3465,12 +3606,15 @@
       <c r="H89">
         <v>14</v>
       </c>
+      <c r="J89">
+        <v>12</v>
+      </c>
       <c r="K89">
         <v>1</v>
       </c>
       <c r="N89">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3509,12 +3653,15 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="6"/>
+      <c r="H91">
+        <v>15</v>
+      </c>
       <c r="K91">
         <v>1</v>
       </c>
       <c r="N91">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3531,12 +3678,18 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="6"/>
+      <c r="H92">
+        <v>15</v>
+      </c>
+      <c r="J92">
+        <v>14</v>
+      </c>
       <c r="K92">
         <v>1</v>
       </c>
       <c r="N92">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3556,12 +3709,15 @@
       <c r="H93">
         <v>14</v>
       </c>
+      <c r="J93">
+        <v>10</v>
+      </c>
       <c r="K93">
         <v>1</v>
       </c>
       <c r="N93">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3581,12 +3737,15 @@
       <c r="H94">
         <v>15</v>
       </c>
+      <c r="J94">
+        <v>12</v>
+      </c>
       <c r="K94">
         <v>1</v>
       </c>
       <c r="N94">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3625,12 +3784,15 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="6"/>
+      <c r="J96">
+        <v>6</v>
+      </c>
       <c r="K96">
         <v>1</v>
       </c>
       <c r="N96">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3647,12 +3809,18 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="6"/>
+      <c r="H97">
+        <v>15</v>
+      </c>
+      <c r="J97">
+        <v>10</v>
+      </c>
       <c r="K97">
         <v>1</v>
       </c>
       <c r="N97">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3672,12 +3840,15 @@
       <c r="H98">
         <v>14</v>
       </c>
+      <c r="J98">
+        <v>10</v>
+      </c>
       <c r="K98">
         <v>1</v>
       </c>
       <c r="N98">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ready con Base de Datos, Felicidades a los que pasaron, mejor suerte al resto
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
+++ b/OYM/_DocumentosComunes/_BD (Autosaved).xlsx
@@ -15,7 +15,7 @@
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$99</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$93</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1194,8 +1194,8 @@
   <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1324,30 +1324,27 @@
         <v>17</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D66" si="0">IF((N3)&gt;=70,10,"")</f>
+        <f>IF((N3)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E66" si="1">IF((N3)&gt;=70,20,"")</f>
+        <f>IF((N3)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F3" s="2" t="str">
-        <f t="shared" ref="F3:F66" si="2">IF((N3)&gt;=70,20,"")</f>
+        <f>IF((N3)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G3" s="6" t="str">
-        <f t="shared" ref="G3:G66" si="3">IF((N3)&gt;=70,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
-        <v/>
-      </c>
-      <c r="I3">
-        <v>10</v>
+        <f>IF((N3)&gt;=70,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
+        <v/>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N66" si="4">IF((H3+I3+J3+L3+M3+O3)&lt;70,IF((H3+I3+J3+L3+M3+O3)&gt;59,70,(H3+I3+J3+L3+M3+O3)),(H3+I3+J3+L3+M3+O3))</f>
-        <v>10</v>
+        <f>IF((H3+I3+J3+L3+M3+O3)&lt;70,IF((H3+I3+J3+L3+M3+O3)&gt;59,70,(H3+I3+J3+L3+M3+O3)),(H3+I3+J3+L3+M3+O3))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1361,30 +1358,27 @@
         <v>19</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N4)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N4)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N4)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G4" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I4">
-        <v>10</v>
+        <f>IF((N4)&gt;=70,IF((N4-50)&gt;50,50,IF((N4-50)&lt;0,0,(N4-50))), "" )</f>
+        <v/>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H4+I4+J4+L4+M4+O4)&lt;70,IF((H4+I4+J4+L4+M4+O4)&gt;59,70,(H4+I4+J4+L4+M4+O4)),(H4+I4+J4+L4+M4+O4))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1398,19 +1392,19 @@
         <v>21</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N5)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N5)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N5)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N5)&gt;=70,IF((N5-50)&gt;50,50,IF((N5-50)&lt;0,0,(N5-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H5">
@@ -1429,7 +1423,7 @@
         <v>15</v>
       </c>
       <c r="N5">
-        <f t="shared" si="4"/>
+        <f>IF((H5+I5+J5+L5+M5+O5)&lt;70,IF((H5+I5+J5+L5+M5+O5)&gt;59,70,(H5+I5+J5+L5+M5+O5)),(H5+I5+J5+L5+M5+O5))</f>
         <v>70</v>
       </c>
     </row>
@@ -1443,24 +1437,21 @@
       <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F6" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G6" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I6">
-        <v>10</v>
+      <c r="D6" s="6">
+        <f>IF((N6)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <f>IF((N6)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
+        <f>IF((N6)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G6" s="6">
+        <f>IF((N6)&gt;=70,IF((N6-50)&gt;50,50,IF((N6-50)&lt;0,0,(N6-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>12</v>
@@ -1471,9 +1462,12 @@
       <c r="L6">
         <v>20</v>
       </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
       <c r="N6">
-        <f t="shared" si="4"/>
-        <v>42</v>
+        <f>IF((H6+I6+J6+L6+M6+O6)&lt;70,IF((H6+I6+J6+L6+M6+O6)&gt;59,70,(H6+I6+J6+L6+M6+O6)),(H6+I6+J6+L6+M6+O6))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1487,19 +1481,19 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N7)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N7)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F7" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N7)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G7" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N7)&gt;=70,IF((N7-50)&gt;50,50,IF((N7-50)&lt;0,0,(N7-50))), "" )</f>
         <v/>
       </c>
       <c r="H7">
@@ -1512,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="4"/>
+        <f>IF((H7+I7+J7+L7+M7+O7)&lt;70,IF((H7+I7+J7+L7+M7+O7)&gt;59,70,(H7+I7+J7+L7+M7+O7)),(H7+I7+J7+L7+M7+O7))</f>
         <v>27</v>
       </c>
     </row>
@@ -1527,30 +1521,27 @@
         <v>27</v>
       </c>
       <c r="D8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N8)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N8)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F8" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N8)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G8" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I8">
-        <v>10</v>
+        <f>IF((N8)&gt;=70,IF((N8-50)&gt;50,50,IF((N8-50)&lt;0,0,(N8-50))), "" )</f>
+        <v/>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="N8">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H8+I8+J8+L8+M8+O8)&lt;70,IF((H8+I8+J8+L8+M8+O8)&gt;59,70,(H8+I8+J8+L8+M8+O8)),(H8+I8+J8+L8+M8+O8))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1563,21 +1554,24 @@
       <c r="C9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F9" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G9" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D9" s="6">
+        <f>IF((N9)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <f>IF((N9)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F9" s="2">
+        <f>IF((N9)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G9" s="6">
+        <f>IF((N9)&gt;=70,IF((N9-50)&gt;50,50,IF((N9-50)&lt;0,0,(N9-50))), "" )</f>
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9">
         <v>10</v>
@@ -1591,9 +1585,12 @@
       <c r="L9">
         <v>20</v>
       </c>
+      <c r="M9">
+        <v>18</v>
+      </c>
       <c r="N9">
-        <f t="shared" si="4"/>
-        <v>42</v>
+        <f>IF((H9+I9+J9+L9+M9+O9)&lt;70,IF((H9+I9+J9+L9+M9+O9)&gt;59,70,(H9+I9+J9+L9+M9+O9)),(H9+I9+J9+L9+M9+O9))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1607,19 +1604,19 @@
         <v>31</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N10)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N10)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N10)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N10)&gt;=70,IF((N10-50)&gt;50,50,IF((N10-50)&lt;0,0,(N10-50))), "" )</f>
         <v>44</v>
       </c>
       <c r="H10">
@@ -1641,7 +1638,7 @@
         <v>26</v>
       </c>
       <c r="N10">
-        <f t="shared" si="4"/>
+        <f>IF((H10+I10+J10+L10+M10+O10)&lt;70,IF((H10+I10+J10+L10+M10+O10)&gt;59,70,(H10+I10+J10+L10+M10+O10)),(H10+I10+J10+L10+M10+O10))</f>
         <v>94</v>
       </c>
     </row>
@@ -1656,19 +1653,19 @@
         <v>33</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N11)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N11)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N11)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N11)&gt;=70,IF((N11-50)&gt;50,50,IF((N11-50)&lt;0,0,(N11-50))), "" )</f>
         <v>30</v>
       </c>
       <c r="H11">
@@ -1690,7 +1687,7 @@
         <v>30</v>
       </c>
       <c r="N11">
-        <f t="shared" si="4"/>
+        <f>IF((H11+I11+J11+L11+M11+O11)&lt;70,IF((H11+I11+J11+L11+M11+O11)&gt;59,70,(H11+I11+J11+L11+M11+O11)),(H11+I11+J11+L11+M11+O11))</f>
         <v>80</v>
       </c>
     </row>
@@ -1705,20 +1702,20 @@
         <v>35</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N12)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N12)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N12)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N12)&gt;=70,IF((N12-50)&gt;50,50,IF((N12-50)&lt;0,0,(N12-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H12">
         <v>18</v>
@@ -1735,9 +1732,12 @@
       <c r="L12">
         <v>14</v>
       </c>
+      <c r="M12">
+        <v>29</v>
+      </c>
       <c r="N12">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H12+I12+J12+L12+M12+O12)&lt;70,IF((H12+I12+J12+L12+M12+O12)&gt;59,70,(H12+I12+J12+L12+M12+O12)),(H12+I12+J12+L12+M12+O12))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,19 +1751,19 @@
         <v>37</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N13)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N13)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N13)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N13)&gt;=70,IF((N13-50)&gt;50,50,IF((N13-50)&lt;0,0,(N13-50))), "" )</f>
         <v>34</v>
       </c>
       <c r="H13">
@@ -1785,7 +1785,7 @@
         <v>21</v>
       </c>
       <c r="N13">
-        <f t="shared" si="4"/>
+        <f>IF((H13+I13+J13+L13+M13+O13)&lt;70,IF((H13+I13+J13+L13+M13+O13)&gt;59,70,(H13+I13+J13+L13+M13+O13)),(H13+I13+J13+L13+M13+O13))</f>
         <v>84</v>
       </c>
     </row>
@@ -1799,21 +1799,21 @@
       <c r="C14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G14" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D14" s="6">
+        <f>IF((N14)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <f>IF((N14)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F14" s="2">
+        <f>IF((N14)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G14" s="6">
+        <f>IF((N14)&gt;=70,IF((N14-50)&gt;50,50,IF((N14-50)&lt;0,0,(N14-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>15</v>
@@ -1830,9 +1830,12 @@
       <c r="L14">
         <v>20</v>
       </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
       <c r="N14">
-        <f t="shared" si="4"/>
-        <v>53</v>
+        <f>IF((H14+I14+J14+L14+M14+O14)&lt;70,IF((H14+I14+J14+L14+M14+O14)&gt;59,70,(H14+I14+J14+L14+M14+O14)),(H14+I14+J14+L14+M14+O14))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1846,19 +1849,19 @@
         <v>41</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N15)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N15)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N15)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N15)&gt;=70,IF((N15-50)&gt;50,50,IF((N15-50)&lt;0,0,(N15-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H15">
@@ -1877,7 +1880,7 @@
         <v>20</v>
       </c>
       <c r="N15">
-        <f t="shared" si="4"/>
+        <f>IF((H15+I15+J15+L15+M15+O15)&lt;70,IF((H15+I15+J15+L15+M15+O15)&gt;59,70,(H15+I15+J15+L15+M15+O15)),(H15+I15+J15+L15+M15+O15))</f>
         <v>70</v>
       </c>
     </row>
@@ -1891,21 +1894,21 @@
       <c r="C16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G16" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D16" s="6">
+        <f>IF((N16)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
+        <f>IF((N16)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F16" s="2">
+        <f>IF((N16)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G16" s="6">
+        <f>IF((N16)&gt;=70,IF((N16-50)&gt;50,50,IF((N16-50)&lt;0,0,(N16-50))), "" )</f>
+        <v>28</v>
       </c>
       <c r="I16">
         <v>10</v>
@@ -1919,9 +1922,12 @@
       <c r="L16">
         <v>20</v>
       </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
       <c r="N16">
-        <f t="shared" si="4"/>
-        <v>48</v>
+        <f>IF((H16+I16+J16+L16+M16+O16)&lt;70,IF((H16+I16+J16+L16+M16+O16)&gt;59,70,(H16+I16+J16+L16+M16+O16)),(H16+I16+J16+L16+M16+O16))</f>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1935,19 +1941,19 @@
         <v>45</v>
       </c>
       <c r="D17" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N17)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N17)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N17)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G17" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N17)&gt;=70,IF((N17-50)&gt;50,50,IF((N17-50)&lt;0,0,(N17-50))), "" )</f>
         <v/>
       </c>
       <c r="I17">
@@ -1963,7 +1969,7 @@
         <v>15</v>
       </c>
       <c r="N17">
-        <f t="shared" si="4"/>
+        <f>IF((H17+I17+J17+L17+M17+O17)&lt;70,IF((H17+I17+J17+L17+M17+O17)&gt;59,70,(H17+I17+J17+L17+M17+O17)),(H17+I17+J17+L17+M17+O17))</f>
         <v>37</v>
       </c>
     </row>
@@ -1978,30 +1984,27 @@
         <v>47</v>
       </c>
       <c r="D18" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N18)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N18)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N18)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G18" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I18">
-        <v>10</v>
+        <f>IF((N18)&gt;=70,IF((N18-50)&gt;50,50,IF((N18-50)&lt;0,0,(N18-50))), "" )</f>
+        <v/>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="N18">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H18+I18+J18+L18+M18+O18)&lt;70,IF((H18+I18+J18+L18+M18+O18)&gt;59,70,(H18+I18+J18+L18+M18+O18)),(H18+I18+J18+L18+M18+O18))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2015,20 +2018,20 @@
         <v>49</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N19)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N19)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N19)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N19)&gt;=70,IF((N19-50)&gt;50,50,IF((N19-50)&lt;0,0,(N19-50))), "" )</f>
+        <v>42</v>
       </c>
       <c r="H19">
         <v>18</v>
@@ -2045,9 +2048,12 @@
       <c r="L19">
         <v>15</v>
       </c>
+      <c r="M19">
+        <v>29</v>
+      </c>
       <c r="N19">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H19+I19+J19+L19+M19+O19)&lt;70,IF((H19+I19+J19+L19+M19+O19)&gt;59,70,(H19+I19+J19+L19+M19+O19)),(H19+I19+J19+L19+M19+O19))</f>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2061,20 +2067,20 @@
         <v>51</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N20)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N20)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N20)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N20)&gt;=70,IF((N20-50)&gt;50,50,IF((N20-50)&lt;0,0,(N20-50))), "" )</f>
+        <v>45</v>
       </c>
       <c r="H20">
         <v>18</v>
@@ -2091,9 +2097,12 @@
       <c r="L20">
         <v>18</v>
       </c>
+      <c r="M20">
+        <v>29</v>
+      </c>
       <c r="N20">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H20+I20+J20+L20+M20+O20)&lt;70,IF((H20+I20+J20+L20+M20+O20)&gt;59,70,(H20+I20+J20+L20+M20+O20)),(H20+I20+J20+L20+M20+O20))</f>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2107,19 +2116,19 @@
         <v>53</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N21)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N21)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N21)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N21)&gt;=70,IF((N21-50)&gt;50,50,IF((N21-50)&lt;0,0,(N21-50))), "" )</f>
         <v>39</v>
       </c>
       <c r="H21">
@@ -2141,7 +2150,7 @@
         <v>21</v>
       </c>
       <c r="N21">
-        <f t="shared" si="4"/>
+        <f>IF((H21+I21+J21+L21+M21+O21)&lt;70,IF((H21+I21+J21+L21+M21+O21)&gt;59,70,(H21+I21+J21+L21+M21+O21)),(H21+I21+J21+L21+M21+O21))</f>
         <v>89</v>
       </c>
     </row>
@@ -2156,19 +2165,19 @@
         <v>55</v>
       </c>
       <c r="D22" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N22)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N22)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N22)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N22)&gt;=70,IF((N22-50)&gt;50,50,IF((N22-50)&lt;0,0,(N22-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="I22">
@@ -2187,7 +2196,7 @@
         <v>15</v>
       </c>
       <c r="N22">
-        <f t="shared" si="4"/>
+        <f>IF((H22+I22+J22+L22+M22+O22)&lt;70,IF((H22+I22+J22+L22+M22+O22)&gt;59,70,(H22+I22+J22+L22+M22+O22)),(H22+I22+J22+L22+M22+O22))</f>
         <v>70</v>
       </c>
     </row>
@@ -2202,30 +2211,27 @@
         <v>57</v>
       </c>
       <c r="D23" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N23)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N23)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N23)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G23" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I23">
-        <v>10</v>
+        <f>IF((N23)&gt;=70,IF((N23-50)&gt;50,50,IF((N23-50)&lt;0,0,(N23-50))), "" )</f>
+        <v/>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="N23">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H23+I23+J23+L23+M23+O23)&lt;70,IF((H23+I23+J23+L23+M23+O23)&gt;59,70,(H23+I23+J23+L23+M23+O23)),(H23+I23+J23+L23+M23+O23))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2239,30 +2245,27 @@
         <v>59</v>
       </c>
       <c r="D24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N24)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N24)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N24)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G24" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I24">
-        <v>10</v>
+        <f>IF((N24)&gt;=70,IF((N24-50)&gt;50,50,IF((N24-50)&lt;0,0,(N24-50))), "" )</f>
+        <v/>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="N24">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H24+I24+J24+L24+M24+O24)&lt;70,IF((H24+I24+J24+L24+M24+O24)&gt;59,70,(H24+I24+J24+L24+M24+O24)),(H24+I24+J24+L24+M24+O24))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2276,30 +2279,27 @@
         <v>61</v>
       </c>
       <c r="D25" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N25)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N25)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N25)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G25" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I25">
-        <v>10</v>
+        <f>IF((N25)&gt;=70,IF((N25-50)&gt;50,50,IF((N25-50)&lt;0,0,(N25-50))), "" )</f>
+        <v/>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H25+I25+J25+L25+M25+O25)&lt;70,IF((H25+I25+J25+L25+M25+O25)&gt;59,70,(H25+I25+J25+L25+M25+O25)),(H25+I25+J25+L25+M25+O25))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,30 +2313,27 @@
         <v>63</v>
       </c>
       <c r="D26" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N26)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N26)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N26)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G26" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I26">
-        <v>10</v>
+        <f>IF((N26)&gt;=70,IF((N26-50)&gt;50,50,IF((N26-50)&lt;0,0,(N26-50))), "" )</f>
+        <v/>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="N26">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H26+I26+J26+L26+M26+O26)&lt;70,IF((H26+I26+J26+L26+M26+O26)&gt;59,70,(H26+I26+J26+L26+M26+O26)),(H26+I26+J26+L26+M26+O26))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2349,21 +2346,21 @@
       <c r="C27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G27" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D27" s="6">
+        <f>IF((N27)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <f>IF((N27)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F27" s="2">
+        <f>IF((N27)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G27" s="6">
+        <f>IF((N27)&gt;=70,IF((N27-50)&gt;50,50,IF((N27-50)&lt;0,0,(N27-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H27">
         <v>15</v>
@@ -2380,9 +2377,12 @@
       <c r="L27">
         <v>20</v>
       </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
       <c r="N27">
-        <f t="shared" si="4"/>
-        <v>59</v>
+        <f>IF((H27+I27+J27+L27+M27+O27)&lt;70,IF((H27+I27+J27+L27+M27+O27)&gt;59,70,(H27+I27+J27+L27+M27+O27)),(H27+I27+J27+L27+M27+O27))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2395,21 +2395,21 @@
       <c r="C28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E28" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F28" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G28" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D28" s="6">
+        <f>IF((N28)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E28" s="2">
+        <f>IF((N28)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F28" s="2">
+        <f>IF((N28)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G28" s="6">
+        <f>IF((N28)&gt;=70,IF((N28-50)&gt;50,50,IF((N28-50)&lt;0,0,(N28-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H28">
         <v>15</v>
@@ -2423,9 +2423,12 @@
       <c r="L28">
         <v>20</v>
       </c>
+      <c r="M28">
+        <v>15</v>
+      </c>
       <c r="N28">
-        <f t="shared" si="4"/>
-        <v>45</v>
+        <f>IF((H28+I28+J28+L28+M28+O28)&lt;70,IF((H28+I28+J28+L28+M28+O28)&gt;59,70,(H28+I28+J28+L28+M28+O28)),(H28+I28+J28+L28+M28+O28))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2438,21 +2441,21 @@
       <c r="C29" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E29" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G29" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D29" s="6">
+        <f>IF((N29)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <f>IF((N29)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F29" s="2">
+        <f>IF((N29)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G29" s="6">
+        <f>IF((N29)&gt;=70,IF((N29-50)&gt;50,50,IF((N29-50)&lt;0,0,(N29-50))), "" )</f>
+        <v>26</v>
       </c>
       <c r="H29">
         <v>15</v>
@@ -2469,9 +2472,12 @@
       <c r="L29">
         <v>20</v>
       </c>
+      <c r="M29">
+        <v>23</v>
+      </c>
       <c r="N29">
-        <f t="shared" si="4"/>
-        <v>53</v>
+        <f>IF((H29+I29+J29+L29+M29+O29)&lt;70,IF((H29+I29+J29+L29+M29+O29)&gt;59,70,(H29+I29+J29+L29+M29+O29)),(H29+I29+J29+L29+M29+O29))</f>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2484,21 +2490,21 @@
       <c r="C30" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E30" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G30" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D30" s="6">
+        <f>IF((N30)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E30" s="2">
+        <f>IF((N30)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F30" s="2">
+        <f>IF((N30)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G30" s="6">
+        <f>IF((N30)&gt;=70,IF((N30-50)&gt;50,50,IF((N30-50)&lt;0,0,(N30-50))), "" )</f>
+        <v>34</v>
       </c>
       <c r="H30">
         <v>15</v>
@@ -2515,9 +2521,12 @@
       <c r="L30">
         <v>20</v>
       </c>
+      <c r="M30">
+        <v>27</v>
+      </c>
       <c r="N30">
-        <f t="shared" si="4"/>
-        <v>57</v>
+        <f>IF((H30+I30+J30+L30+M30+O30)&lt;70,IF((H30+I30+J30+L30+M30+O30)&gt;59,70,(H30+I30+J30+L30+M30+O30)),(H30+I30+J30+L30+M30+O30))</f>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2530,21 +2539,21 @@
       <c r="C31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E31" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G31" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D31" s="6">
+        <f>IF((N31)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E31" s="2">
+        <f>IF((N31)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F31" s="2">
+        <f>IF((N31)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G31" s="6">
+        <f>IF((N31)&gt;=70,IF((N31-50)&gt;50,50,IF((N31-50)&lt;0,0,(N31-50))), "" )</f>
+        <v>34</v>
       </c>
       <c r="H31">
         <v>17</v>
@@ -2561,9 +2570,12 @@
       <c r="L31">
         <v>15</v>
       </c>
+      <c r="M31">
+        <v>30</v>
+      </c>
       <c r="N31">
-        <f t="shared" si="4"/>
-        <v>54</v>
+        <f>IF((H31+I31+J31+L31+M31+O31)&lt;70,IF((H31+I31+J31+L31+M31+O31)&gt;59,70,(H31+I31+J31+L31+M31+O31)),(H31+I31+J31+L31+M31+O31))</f>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2576,21 +2588,21 @@
       <c r="C32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E32" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F32" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G32" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D32" s="6">
+        <f>IF((N32)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E32" s="2">
+        <f>IF((N32)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F32" s="2">
+        <f>IF((N32)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G32" s="6">
+        <f>IF((N32)&gt;=70,IF((N32-50)&gt;50,50,IF((N32-50)&lt;0,0,(N32-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H32">
         <v>15</v>
@@ -2607,9 +2619,12 @@
       <c r="L32">
         <v>20</v>
       </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
       <c r="N32">
-        <f t="shared" si="4"/>
-        <v>59</v>
+        <f>IF((H32+I32+J32+L32+M32+O32)&lt;70,IF((H32+I32+J32+L32+M32+O32)&gt;59,70,(H32+I32+J32+L32+M32+O32)),(H32+I32+J32+L32+M32+O32))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2623,19 +2638,19 @@
         <v>77</v>
       </c>
       <c r="D33" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N33)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E33" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N33)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N33)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G33" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N33)&gt;=70,IF((N33-50)&gt;50,50,IF((N33-50)&lt;0,0,(N33-50))), "" )</f>
         <v/>
       </c>
       <c r="H33">
@@ -2651,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="N33">
-        <f t="shared" si="4"/>
+        <f>IF((H33+I33+J33+L33+M33+O33)&lt;70,IF((H33+I33+J33+L33+M33+O33)&gt;59,70,(H33+I33+J33+L33+M33+O33)),(H33+I33+J33+L33+M33+O33))</f>
         <v>37</v>
       </c>
     </row>
@@ -2666,19 +2681,19 @@
         <v>79</v>
       </c>
       <c r="D34" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N34)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N34)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N34)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G34" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N34)&gt;=70,IF((N34-50)&gt;50,50,IF((N34-50)&lt;0,0,(N34-50))), "" )</f>
         <v/>
       </c>
       <c r="H34">
@@ -2691,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="N34">
-        <f t="shared" si="4"/>
+        <f>IF((H34+I34+J34+L34+M34+O34)&lt;70,IF((H34+I34+J34+L34+M34+O34)&gt;59,70,(H34+I34+J34+L34+M34+O34)),(H34+I34+J34+L34+M34+O34))</f>
         <v>25</v>
       </c>
     </row>
@@ -2706,20 +2721,20 @@
         <v>81</v>
       </c>
       <c r="D35" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N35)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N35)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N35)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G35" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N35)&gt;=70,IF((N35-50)&gt;50,50,IF((N35-50)&lt;0,0,(N35-50))), "" )</f>
+        <v>46</v>
       </c>
       <c r="H35">
         <v>18</v>
@@ -2736,9 +2751,12 @@
       <c r="L35">
         <v>20</v>
       </c>
+      <c r="M35">
+        <v>28</v>
+      </c>
       <c r="N35">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H35+I35+J35+L35+M35+O35)&lt;70,IF((H35+I35+J35+L35+M35+O35)&gt;59,70,(H35+I35+J35+L35+M35+O35)),(H35+I35+J35+L35+M35+O35))</f>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2752,19 +2770,19 @@
         <v>83</v>
       </c>
       <c r="D36" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N36)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N36)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N36)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G36" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N36)&gt;=70,IF((N36-50)&gt;50,50,IF((N36-50)&lt;0,0,(N36-50))), "" )</f>
         <v>36</v>
       </c>
       <c r="H36">
@@ -2786,7 +2804,7 @@
         <v>25</v>
       </c>
       <c r="N36">
-        <f t="shared" si="4"/>
+        <f>IF((H36+I36+J36+L36+M36+O36)&lt;70,IF((H36+I36+J36+L36+M36+O36)&gt;59,70,(H36+I36+J36+L36+M36+O36)),(H36+I36+J36+L36+M36+O36))</f>
         <v>86</v>
       </c>
     </row>
@@ -2801,19 +2819,19 @@
         <v>85</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N37)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N37)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N37)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G37" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N37)&gt;=70,IF((N37-50)&gt;50,50,IF((N37-50)&lt;0,0,(N37-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H37">
@@ -2835,7 +2853,7 @@
         <v>29</v>
       </c>
       <c r="N37">
-        <f t="shared" si="4"/>
+        <f>IF((H37+I37+J37+L37+M37+O37)&lt;70,IF((H37+I37+J37+L37+M37+O37)&gt;59,70,(H37+I37+J37+L37+M37+O37)),(H37+I37+J37+L37+M37+O37))</f>
         <v>93</v>
       </c>
     </row>
@@ -2850,19 +2868,19 @@
         <v>87</v>
       </c>
       <c r="D38" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N38)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E38" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N38)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N38)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G38" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N38)&gt;=70,IF((N38-50)&gt;50,50,IF((N38-50)&lt;0,0,(N38-50))), "" )</f>
         <v/>
       </c>
       <c r="H38">
@@ -2878,7 +2896,7 @@
         <v>25</v>
       </c>
       <c r="N38">
-        <f t="shared" si="4"/>
+        <f>IF((H38+I38+J38+L38+M38+O38)&lt;70,IF((H38+I38+J38+L38+M38+O38)&gt;59,70,(H38+I38+J38+L38+M38+O38)),(H38+I38+J38+L38+M38+O38))</f>
         <v>53</v>
       </c>
     </row>
@@ -2893,19 +2911,19 @@
         <v>89</v>
       </c>
       <c r="D39" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N39)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E39" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N39)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F39" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N39)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G39" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N39)&gt;=70,IF((N39-50)&gt;50,50,IF((N39-50)&lt;0,0,(N39-50))), "" )</f>
         <v/>
       </c>
       <c r="H39">
@@ -2924,7 +2942,7 @@
         <v>15</v>
       </c>
       <c r="N39">
-        <f t="shared" si="4"/>
+        <f>IF((H39+I39+J39+L39+M39+O39)&lt;70,IF((H39+I39+J39+L39+M39+O39)&gt;59,70,(H39+I39+J39+L39+M39+O39)),(H39+I39+J39+L39+M39+O39))</f>
         <v>52</v>
       </c>
     </row>
@@ -2939,19 +2957,19 @@
         <v>91</v>
       </c>
       <c r="D40" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N40)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E40" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N40)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F40" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N40)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G40" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N40)&gt;=70,IF((N40-50)&gt;50,50,IF((N40-50)&lt;0,0,(N40-50))), "" )</f>
         <v/>
       </c>
       <c r="I40">
@@ -2961,7 +2979,7 @@
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" si="4"/>
+        <f>IF((H40+I40+J40+L40+M40+O40)&lt;70,IF((H40+I40+J40+L40+M40+O40)&gt;59,70,(H40+I40+J40+L40+M40+O40)),(H40+I40+J40+L40+M40+O40))</f>
         <v>10</v>
       </c>
     </row>
@@ -2976,19 +2994,19 @@
         <v>93</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N41)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N41)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N41)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N41)&gt;=70,IF((N41-50)&gt;50,50,IF((N41-50)&lt;0,0,(N41-50))), "" )</f>
         <v>39</v>
       </c>
       <c r="H41">
@@ -3010,7 +3028,7 @@
         <v>29</v>
       </c>
       <c r="N41">
-        <f t="shared" si="4"/>
+        <f>IF((H41+I41+J41+L41+M41+O41)&lt;70,IF((H41+I41+J41+L41+M41+O41)&gt;59,70,(H41+I41+J41+L41+M41+O41)),(H41+I41+J41+L41+M41+O41))</f>
         <v>89</v>
       </c>
     </row>
@@ -3025,20 +3043,20 @@
         <v>95</v>
       </c>
       <c r="D42" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N42)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N42)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N42)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G42" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N42)&gt;=70,IF((N42-50)&gt;50,50,IF((N42-50)&lt;0,0,(N42-50))), "" )</f>
+        <v>48</v>
       </c>
       <c r="H42">
         <v>18</v>
@@ -3055,9 +3073,12 @@
       <c r="L42">
         <v>20</v>
       </c>
+      <c r="M42">
+        <v>30</v>
+      </c>
       <c r="N42">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H42+I42+J42+L42+M42+O42)&lt;70,IF((H42+I42+J42+L42+M42+O42)&gt;59,70,(H42+I42+J42+L42+M42+O42)),(H42+I42+J42+L42+M42+O42))</f>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3071,19 +3092,19 @@
         <v>97</v>
       </c>
       <c r="D43" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N43)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N43)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N43)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N43)&gt;=70,IF((N43-50)&gt;50,50,IF((N43-50)&lt;0,0,(N43-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H43">
@@ -3105,7 +3126,7 @@
         <v>25</v>
       </c>
       <c r="N43">
-        <f t="shared" si="4"/>
+        <f>IF((H43+I43+J43+L43+M43+O43)&lt;70,IF((H43+I43+J43+L43+M43+O43)&gt;59,70,(H43+I43+J43+L43+M43+O43)),(H43+I43+J43+L43+M43+O43))</f>
         <v>93</v>
       </c>
     </row>
@@ -3120,19 +3141,19 @@
         <v>99</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N44)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N44)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N44)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N44)&gt;=70,IF((N44-50)&gt;50,50,IF((N44-50)&lt;0,0,(N44-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H44">
@@ -3154,7 +3175,7 @@
         <v>25</v>
       </c>
       <c r="N44">
-        <f t="shared" si="4"/>
+        <f>IF((H44+I44+J44+L44+M44+O44)&lt;70,IF((H44+I44+J44+L44+M44+O44)&gt;59,70,(H44+I44+J44+L44+M44+O44)),(H44+I44+J44+L44+M44+O44))</f>
         <v>93</v>
       </c>
     </row>
@@ -3168,21 +3189,21 @@
       <c r="C45" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E45" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G45" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D45" s="6">
+        <f>IF((N45)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E45" s="2">
+        <f>IF((N45)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F45" s="2">
+        <f>IF((N45)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G45" s="6">
+        <f>IF((N45)&gt;=70,IF((N45-50)&gt;50,50,IF((N45-50)&lt;0,0,(N45-50))), "" )</f>
+        <v>30</v>
       </c>
       <c r="H45">
         <v>17</v>
@@ -3199,9 +3220,12 @@
       <c r="L45">
         <v>15</v>
       </c>
+      <c r="M45">
+        <v>30</v>
+      </c>
       <c r="N45">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f>IF((H45+I45+J45+L45+M45+O45)&lt;70,IF((H45+I45+J45+L45+M45+O45)&gt;59,70,(H45+I45+J45+L45+M45+O45)),(H45+I45+J45+L45+M45+O45))</f>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3215,19 +3239,19 @@
         <v>103</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N46)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N46)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N46)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N46)&gt;=70,IF((N46-50)&gt;50,50,IF((N46-50)&lt;0,0,(N46-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H46">
@@ -3249,7 +3273,7 @@
         <v>15</v>
       </c>
       <c r="N46">
-        <f t="shared" si="4"/>
+        <f>IF((H46+I46+J46+L46+M46+O46)&lt;70,IF((H46+I46+J46+L46+M46+O46)&gt;59,70,(H46+I46+J46+L46+M46+O46)),(H46+I46+J46+L46+M46+O46))</f>
         <v>70</v>
       </c>
     </row>
@@ -3263,21 +3287,21 @@
       <c r="C47" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E47" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G47" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D47" s="6">
+        <f>IF((N47)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E47" s="2">
+        <f>IF((N47)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F47" s="2">
+        <f>IF((N47)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G47" s="6">
+        <f>IF((N47)&gt;=70,IF((N47-50)&gt;50,50,IF((N47-50)&lt;0,0,(N47-50))), "" )</f>
+        <v>39</v>
       </c>
       <c r="H47">
         <v>18</v>
@@ -3294,9 +3318,12 @@
       <c r="L47">
         <v>20</v>
       </c>
+      <c r="M47">
+        <v>30</v>
+      </c>
       <c r="N47">
-        <f t="shared" si="4"/>
-        <v>59</v>
+        <f>IF((H47+I47+J47+L47+M47+O47)&lt;70,IF((H47+I47+J47+L47+M47+O47)&gt;59,70,(H47+I47+J47+L47+M47+O47)),(H47+I47+J47+L47+M47+O47))</f>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3310,19 +3337,19 @@
         <v>107</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N48)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N48)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N48)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G48" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N48)&gt;=70,IF((N48-50)&gt;50,50,IF((N48-50)&lt;0,0,(N48-50))), "" )</f>
         <v>41</v>
       </c>
       <c r="H48">
@@ -3344,7 +3371,7 @@
         <v>30</v>
       </c>
       <c r="N48">
-        <f t="shared" si="4"/>
+        <f>IF((H48+I48+J48+L48+M48+O48)&lt;70,IF((H48+I48+J48+L48+M48+O48)&gt;59,70,(H48+I48+J48+L48+M48+O48)),(H48+I48+J48+L48+M48+O48))</f>
         <v>91</v>
       </c>
     </row>
@@ -3359,30 +3386,27 @@
         <v>109</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N49)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E49" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N49)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F49" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N49)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G49" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I49">
-        <v>10</v>
+        <f>IF((N49)&gt;=70,IF((N49-50)&gt;50,50,IF((N49-50)&lt;0,0,(N49-50))), "" )</f>
+        <v/>
       </c>
       <c r="K49">
         <v>1</v>
       </c>
       <c r="N49">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>IF((H49+I49+J49+L49+M49+O49)&lt;70,IF((H49+I49+J49+L49+M49+O49)&gt;59,70,(H49+I49+J49+L49+M49+O49)),(H49+I49+J49+L49+M49+O49))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3396,20 +3420,20 @@
         <v>111</v>
       </c>
       <c r="D50" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N50)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N50)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N50)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G50" s="6">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f>IF((N50)&gt;=70,IF((N50-50)&gt;50,50,IF((N50-50)&lt;0,0,(N50-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H50">
         <v>17</v>
@@ -3427,11 +3451,11 @@
         <v>20</v>
       </c>
       <c r="M50">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="N50">
-        <f t="shared" si="4"/>
-        <v>76</v>
+        <f>IF((H50+I50+J50+L50+M50+O50)&lt;70,IF((H50+I50+J50+L50+M50+O50)&gt;59,70,(H50+I50+J50+L50+M50+O50)),(H50+I50+J50+L50+M50+O50))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3445,19 +3469,19 @@
         <v>113</v>
       </c>
       <c r="D51" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N51)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N51)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N51)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G51" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N51)&gt;=70,IF((N51-50)&gt;50,50,IF((N51-50)&lt;0,0,(N51-50))), "" )</f>
         <v>28</v>
       </c>
       <c r="H51">
@@ -3479,7 +3503,7 @@
         <v>25</v>
       </c>
       <c r="N51">
-        <f t="shared" si="4"/>
+        <f>IF((H51+I51+J51+L51+M51+O51)&lt;70,IF((H51+I51+J51+L51+M51+O51)&gt;59,70,(H51+I51+J51+L51+M51+O51)),(H51+I51+J51+L51+M51+O51))</f>
         <v>78</v>
       </c>
     </row>
@@ -3493,21 +3517,21 @@
       <c r="C52" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E52" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G52" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D52" s="6">
+        <f>IF((N52)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E52" s="2">
+        <f>IF((N52)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F52" s="2">
+        <f>IF((N52)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G52" s="6">
+        <f>IF((N52)&gt;=70,IF((N52-50)&gt;50,50,IF((N52-50)&lt;0,0,(N52-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H52">
         <v>15</v>
@@ -3524,9 +3548,12 @@
       <c r="L52">
         <v>20</v>
       </c>
+      <c r="M52">
+        <v>9</v>
+      </c>
       <c r="N52">
-        <f t="shared" si="4"/>
-        <v>51</v>
+        <f>IF((H52+I52+J52+L52+M52+O52)&lt;70,IF((H52+I52+J52+L52+M52+O52)&gt;59,70,(H52+I52+J52+L52+M52+O52)),(H52+I52+J52+L52+M52+O52))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3540,19 +3567,19 @@
         <v>117</v>
       </c>
       <c r="D53" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N53)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N53)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N53)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G53" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N53)&gt;=70,IF((N53-50)&gt;50,50,IF((N53-50)&lt;0,0,(N53-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="I53">
@@ -3571,7 +3598,7 @@
         <v>25</v>
       </c>
       <c r="N53">
-        <f t="shared" si="4"/>
+        <f>IF((H53+I53+J53+L53+M53+O53)&lt;70,IF((H53+I53+J53+L53+M53+O53)&gt;59,70,(H53+I53+J53+L53+M53+O53)),(H53+I53+J53+L53+M53+O53))</f>
         <v>70</v>
       </c>
     </row>
@@ -3586,19 +3613,19 @@
         <v>119</v>
       </c>
       <c r="D54" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N54)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N54)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N54)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G54" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N54)&gt;=70,IF((N54-50)&gt;50,50,IF((N54-50)&lt;0,0,(N54-50))), "" )</f>
         <v>37</v>
       </c>
       <c r="H54">
@@ -3620,7 +3647,7 @@
         <v>29</v>
       </c>
       <c r="N54">
-        <f t="shared" si="4"/>
+        <f>IF((H54+I54+J54+L54+M54+O54)&lt;70,IF((H54+I54+J54+L54+M54+O54)&gt;59,70,(H54+I54+J54+L54+M54+O54)),(H54+I54+J54+L54+M54+O54))</f>
         <v>87</v>
       </c>
     </row>
@@ -3635,19 +3662,19 @@
         <v>121</v>
       </c>
       <c r="D55" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N55)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E55" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N55)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F55" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N55)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G55" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N55)&gt;=70,IF((N55-50)&gt;50,50,IF((N55-50)&lt;0,0,(N55-50))), "" )</f>
         <v/>
       </c>
       <c r="H55">
@@ -3663,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="N55">
-        <f t="shared" si="4"/>
+        <f>IF((H55+I55+J55+L55+M55+O55)&lt;70,IF((H55+I55+J55+L55+M55+O55)&gt;59,70,(H55+I55+J55+L55+M55+O55)),(H55+I55+J55+L55+M55+O55))</f>
         <v>37</v>
       </c>
     </row>
@@ -3678,19 +3705,19 @@
         <v>123</v>
       </c>
       <c r="D56" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N56)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N56)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N56)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G56" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N56)&gt;=70,IF((N56-50)&gt;50,50,IF((N56-50)&lt;0,0,(N56-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H56">
@@ -3709,7 +3736,7 @@
         <v>30</v>
       </c>
       <c r="N56">
-        <f t="shared" si="4"/>
+        <f>IF((H56+I56+J56+L56+M56+O56)&lt;70,IF((H56+I56+J56+L56+M56+O56)&gt;59,70,(H56+I56+J56+L56+M56+O56)),(H56+I56+J56+L56+M56+O56))</f>
         <v>70</v>
       </c>
     </row>
@@ -3724,19 +3751,19 @@
         <v>125</v>
       </c>
       <c r="D57" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N57)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E57" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N57)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F57" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N57)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G57" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N57)&gt;=70,IF((N57-50)&gt;50,50,IF((N57-50)&lt;0,0,(N57-50))), "" )</f>
         <v/>
       </c>
       <c r="I57">
@@ -3746,7 +3773,7 @@
         <v>1</v>
       </c>
       <c r="N57">
-        <f t="shared" si="4"/>
+        <f>IF((H57+I57+J57+L57+M57+O57)&lt;70,IF((H57+I57+J57+L57+M57+O57)&gt;59,70,(H57+I57+J57+L57+M57+O57)),(H57+I57+J57+L57+M57+O57))</f>
         <v>10</v>
       </c>
     </row>
@@ -3761,19 +3788,19 @@
         <v>127</v>
       </c>
       <c r="D58" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N58)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E58" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N58)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F58" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N58)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G58" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N58)&gt;=70,IF((N58-50)&gt;50,50,IF((N58-50)&lt;0,0,(N58-50))), "" )</f>
         <v/>
       </c>
       <c r="H58">
@@ -3792,7 +3819,7 @@
         <v>15</v>
       </c>
       <c r="N58">
-        <f t="shared" si="4"/>
+        <f>IF((H58+I58+J58+L58+M58+O58)&lt;70,IF((H58+I58+J58+L58+M58+O58)&gt;59,70,(H58+I58+J58+L58+M58+O58)),(H58+I58+J58+L58+M58+O58))</f>
         <v>52</v>
       </c>
     </row>
@@ -3807,19 +3834,19 @@
         <v>129</v>
       </c>
       <c r="D59" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N59)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E59" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N59)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F59" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N59)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G59" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N59)&gt;=70,IF((N59-50)&gt;50,50,IF((N59-50)&lt;0,0,(N59-50))), "" )</f>
         <v/>
       </c>
       <c r="H59">
@@ -3835,7 +3862,7 @@
         <v>14</v>
       </c>
       <c r="N59">
-        <f t="shared" si="4"/>
+        <f>IF((H59+I59+J59+L59+M59+O59)&lt;70,IF((H59+I59+J59+L59+M59+O59)&gt;59,70,(H59+I59+J59+L59+M59+O59)),(H59+I59+J59+L59+M59+O59))</f>
         <v>39</v>
       </c>
     </row>
@@ -3850,19 +3877,19 @@
         <v>131</v>
       </c>
       <c r="D60" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N60)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E60" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N60)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F60" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N60)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G60" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N60)&gt;=70,IF((N60-50)&gt;50,50,IF((N60-50)&lt;0,0,(N60-50))), "" )</f>
         <v/>
       </c>
       <c r="H60">
@@ -3878,7 +3905,7 @@
         <v>15</v>
       </c>
       <c r="N60">
-        <f t="shared" si="4"/>
+        <f>IF((H60+I60+J60+L60+M60+O60)&lt;70,IF((H60+I60+J60+L60+M60+O60)&gt;59,70,(H60+I60+J60+L60+M60+O60)),(H60+I60+J60+L60+M60+O60))</f>
         <v>40</v>
       </c>
     </row>
@@ -3893,19 +3920,19 @@
         <v>133</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N61)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E61" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N61)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F61" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N61)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G61" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N61)&gt;=70,IF((N61-50)&gt;50,50,IF((N61-50)&lt;0,0,(N61-50))), "" )</f>
         <v/>
       </c>
       <c r="H61">
@@ -3924,7 +3951,7 @@
         <v>15</v>
       </c>
       <c r="N61">
-        <f t="shared" si="4"/>
+        <f>IF((H61+I61+J61+L61+M61+O61)&lt;70,IF((H61+I61+J61+L61+M61+O61)&gt;59,70,(H61+I61+J61+L61+M61+O61)),(H61+I61+J61+L61+M61+O61))</f>
         <v>56</v>
       </c>
     </row>
@@ -3939,19 +3966,19 @@
         <v>135</v>
       </c>
       <c r="D62" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N62)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N62)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F62" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N62)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G62" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N62)&gt;=70,IF((N62-50)&gt;50,50,IF((N62-50)&lt;0,0,(N62-50))), "" )</f>
         <v>21</v>
       </c>
       <c r="H62">
@@ -3973,7 +4000,7 @@
         <v>15</v>
       </c>
       <c r="N62">
-        <f t="shared" si="4"/>
+        <f>IF((H62+I62+J62+L62+M62+O62)&lt;70,IF((H62+I62+J62+L62+M62+O62)&gt;59,70,(H62+I62+J62+L62+M62+O62)),(H62+I62+J62+L62+M62+O62))</f>
         <v>71</v>
       </c>
     </row>
@@ -3988,19 +4015,19 @@
         <v>137</v>
       </c>
       <c r="D63" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N63)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N63)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F63" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N63)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N63)&gt;=70,IF((N63-50)&gt;50,50,IF((N63-50)&lt;0,0,(N63-50))), "" )</f>
         <v>34</v>
       </c>
       <c r="H63">
@@ -4022,7 +4049,7 @@
         <v>28</v>
       </c>
       <c r="N63">
-        <f t="shared" si="4"/>
+        <f>IF((H63+I63+J63+L63+M63+O63)&lt;70,IF((H63+I63+J63+L63+M63+O63)&gt;59,70,(H63+I63+J63+L63+M63+O63)),(H63+I63+J63+L63+M63+O63))</f>
         <v>84</v>
       </c>
     </row>
@@ -4037,19 +4064,19 @@
         <v>139</v>
       </c>
       <c r="D64" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N64)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N64)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F64" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N64)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G64" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N64)&gt;=70,IF((N64-50)&gt;50,50,IF((N64-50)&lt;0,0,(N64-50))), "" )</f>
         <v>32</v>
       </c>
       <c r="H64">
@@ -4071,7 +4098,7 @@
         <v>28</v>
       </c>
       <c r="N64">
-        <f t="shared" si="4"/>
+        <f>IF((H64+I64+J64+L64+M64+O64)&lt;70,IF((H64+I64+J64+L64+M64+O64)&gt;59,70,(H64+I64+J64+L64+M64+O64)),(H64+I64+J64+L64+M64+O64))</f>
         <v>82</v>
       </c>
     </row>
@@ -4085,21 +4112,21 @@
       <c r="C65" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D65" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E65" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G65" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D65" s="6">
+        <f>IF((N65)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E65" s="2">
+        <f>IF((N65)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F65" s="2">
+        <f>IF((N65)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G65" s="6">
+        <f>IF((N65)&gt;=70,IF((N65-50)&gt;50,50,IF((N65-50)&lt;0,0,(N65-50))), "" )</f>
+        <v>32</v>
       </c>
       <c r="H65">
         <v>17</v>
@@ -4116,9 +4143,12 @@
       <c r="L65">
         <v>13</v>
       </c>
+      <c r="M65">
+        <v>30</v>
+      </c>
       <c r="N65">
-        <f t="shared" si="4"/>
-        <v>52</v>
+        <f>IF((H65+I65+J65+L65+M65+O65)&lt;70,IF((H65+I65+J65+L65+M65+O65)&gt;59,70,(H65+I65+J65+L65+M65+O65)),(H65+I65+J65+L65+M65+O65))</f>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4132,19 +4162,19 @@
         <v>143</v>
       </c>
       <c r="D66" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N66)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E66" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N66)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F66" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N66)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G66" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N66)&gt;=70,IF((N66-50)&gt;50,50,IF((N66-50)&lt;0,0,(N66-50))), "" )</f>
         <v/>
       </c>
       <c r="H66">
@@ -4160,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="N66">
-        <f t="shared" si="4"/>
+        <f>IF((H66+I66+J66+L66+M66+O66)&lt;70,IF((H66+I66+J66+L66+M66+O66)&gt;59,70,(H66+I66+J66+L66+M66+O66)),(H66+I66+J66+L66+M66+O66))</f>
         <v>34</v>
       </c>
     </row>
@@ -4175,19 +4205,19 @@
         <v>145</v>
       </c>
       <c r="D67" s="6">
-        <f t="shared" ref="D67:D99" si="5">IF((N67)&gt;=70,10,"")</f>
+        <f>IF((N67)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E99" si="6">IF((N67)&gt;=70,20,"")</f>
+        <f>IF((N67)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F67" s="2">
-        <f t="shared" ref="F67:F99" si="7">IF((N67)&gt;=70,20,"")</f>
+        <f>IF((N67)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G67" s="6">
-        <f t="shared" ref="G67:G99" si="8">IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
+        <f>IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H67">
@@ -4206,7 +4236,7 @@
         <v>30</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N99" si="9">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
+        <f>IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
         <v>70</v>
       </c>
     </row>
@@ -4221,19 +4251,19 @@
         <v>147</v>
       </c>
       <c r="D68" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N68)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E68" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N68)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F68" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N68)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G68" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N68)&gt;=70,IF((N68-50)&gt;50,50,IF((N68-50)&lt;0,0,(N68-50))), "" )</f>
         <v/>
       </c>
       <c r="H68">
@@ -4249,7 +4279,7 @@
         <v>1</v>
       </c>
       <c r="N68">
-        <f t="shared" si="9"/>
+        <f>IF((H68+I68+J68+L68+M68+O68)&lt;70,IF((H68+I68+J68+L68+M68+O68)&gt;59,70,(H68+I68+J68+L68+M68+O68)),(H68+I68+J68+L68+M68+O68))</f>
         <v>35</v>
       </c>
     </row>
@@ -4264,19 +4294,19 @@
         <v>149</v>
       </c>
       <c r="D69" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N69)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E69" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N69)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F69" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N69)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G69" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N69)&gt;=70,IF((N69-50)&gt;50,50,IF((N69-50)&lt;0,0,(N69-50))), "" )</f>
         <v/>
       </c>
       <c r="H69">
@@ -4295,7 +4325,7 @@
         <v>15</v>
       </c>
       <c r="N69">
-        <f t="shared" si="9"/>
+        <f>IF((H69+I69+J69+L69+M69+O69)&lt;70,IF((H69+I69+J69+L69+M69+O69)&gt;59,70,(H69+I69+J69+L69+M69+O69)),(H69+I69+J69+L69+M69+O69))</f>
         <v>50</v>
       </c>
     </row>
@@ -4310,19 +4340,19 @@
         <v>151</v>
       </c>
       <c r="D70" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N70)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E70" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N70)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F70" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N70)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G70" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N70)&gt;=70,IF((N70-50)&gt;50,50,IF((N70-50)&lt;0,0,(N70-50))), "" )</f>
         <v/>
       </c>
       <c r="H70">
@@ -4338,7 +4368,7 @@
         <v>1</v>
       </c>
       <c r="N70">
-        <f t="shared" si="9"/>
+        <f>IF((H70+I70+J70+L70+M70+O70)&lt;70,IF((H70+I70+J70+L70+M70+O70)&gt;59,70,(H70+I70+J70+L70+M70+O70)),(H70+I70+J70+L70+M70+O70))</f>
         <v>38</v>
       </c>
     </row>
@@ -4353,20 +4383,20 @@
         <v>153</v>
       </c>
       <c r="D71" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N71)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N71)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F71" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N71)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G71" s="6">
-        <f t="shared" si="8"/>
-        <v>48</v>
+        <f>IF((N71)&gt;=70,IF((N71-50)&gt;50,50,IF((N71-50)&lt;0,0,(N71-50))), "" )</f>
+        <v>50</v>
       </c>
       <c r="H71">
         <v>23</v>
@@ -4384,11 +4414,11 @@
         <v>20</v>
       </c>
       <c r="M71">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N71">
-        <f t="shared" si="9"/>
-        <v>98</v>
+        <f>IF((H71+I71+J71+L71+M71+O71)&lt;70,IF((H71+I71+J71+L71+M71+O71)&gt;59,70,(H71+I71+J71+L71+M71+O71)),(H71+I71+J71+L71+M71+O71))</f>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4402,20 +4432,20 @@
         <v>155</v>
       </c>
       <c r="D72" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N72)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N72)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F72" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N72)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G72" s="6">
-        <f t="shared" si="8"/>
-        <v>23</v>
+        <f>IF((N72)&gt;=70,IF((N72-50)&gt;50,50,IF((N72-50)&lt;0,0,(N72-50))), "" )</f>
+        <v>50</v>
       </c>
       <c r="H72">
         <v>23</v>
@@ -4432,9 +4462,12 @@
       <c r="L72">
         <v>20</v>
       </c>
+      <c r="M72">
+        <v>30</v>
+      </c>
       <c r="N72">
-        <f t="shared" si="9"/>
-        <v>73</v>
+        <f>IF((H72+I72+J72+L72+M72+O72)&lt;70,IF((H72+I72+J72+L72+M72+O72)&gt;59,70,(H72+I72+J72+L72+M72+O72)),(H72+I72+J72+L72+M72+O72))</f>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4448,19 +4481,19 @@
         <v>157</v>
       </c>
       <c r="D73" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N73)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E73" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N73)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F73" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N73)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G73" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N73)&gt;=70,IF((N73-50)&gt;50,50,IF((N73-50)&lt;0,0,(N73-50))), "" )</f>
         <v>35</v>
       </c>
       <c r="H73">
@@ -4482,7 +4515,7 @@
         <v>30</v>
       </c>
       <c r="N73">
-        <f t="shared" si="9"/>
+        <f>IF((H73+I73+J73+L73+M73+O73)&lt;70,IF((H73+I73+J73+L73+M73+O73)&gt;59,70,(H73+I73+J73+L73+M73+O73)),(H73+I73+J73+L73+M73+O73))</f>
         <v>85</v>
       </c>
     </row>
@@ -4496,21 +4529,21 @@
       <c r="C74" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D74" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E74" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G74" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D74" s="6">
+        <f>IF((N74)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E74" s="2">
+        <f>IF((N74)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F74" s="2">
+        <f>IF((N74)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G74" s="6">
+        <f>IF((N74)&gt;=70,IF((N74-50)&gt;50,50,IF((N74-50)&lt;0,0,(N74-50))), "" )</f>
+        <v>21</v>
       </c>
       <c r="H74">
         <v>18</v>
@@ -4524,9 +4557,12 @@
       <c r="K74">
         <v>1</v>
       </c>
+      <c r="M74">
+        <v>23</v>
+      </c>
       <c r="N74">
-        <f t="shared" si="9"/>
-        <v>48</v>
+        <f>IF((H74+I74+J74+L74+M74+O74)&lt;70,IF((H74+I74+J74+L74+M74+O74)&gt;59,70,(H74+I74+J74+L74+M74+O74)),(H74+I74+J74+L74+M74+O74))</f>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4540,19 +4576,19 @@
         <v>161</v>
       </c>
       <c r="D75" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N75)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N75)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F75" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N75)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G75" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N75)&gt;=70,IF((N75-50)&gt;50,50,IF((N75-50)&lt;0,0,(N75-50))), "" )</f>
         <v>31</v>
       </c>
       <c r="H75">
@@ -4574,7 +4610,7 @@
         <v>29</v>
       </c>
       <c r="N75">
-        <f t="shared" si="9"/>
+        <f>IF((H75+I75+J75+L75+M75+O75)&lt;70,IF((H75+I75+J75+L75+M75+O75)&gt;59,70,(H75+I75+J75+L75+M75+O75)),(H75+I75+J75+L75+M75+O75))</f>
         <v>81</v>
       </c>
     </row>
@@ -4589,19 +4625,19 @@
         <v>163</v>
       </c>
       <c r="D76" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N76)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E76" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N76)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F76" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N76)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G76" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N76)&gt;=70,IF((N76-50)&gt;50,50,IF((N76-50)&lt;0,0,(N76-50))), "" )</f>
         <v>29</v>
       </c>
       <c r="H76">
@@ -4623,7 +4659,7 @@
         <v>25</v>
       </c>
       <c r="N76">
-        <f t="shared" si="9"/>
+        <f>IF((H76+I76+J76+L76+M76+O76)&lt;70,IF((H76+I76+J76+L76+M76+O76)&gt;59,70,(H76+I76+J76+L76+M76+O76)),(H76+I76+J76+L76+M76+O76))</f>
         <v>79</v>
       </c>
     </row>
@@ -4638,19 +4674,19 @@
         <v>165</v>
       </c>
       <c r="D77" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N77)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E77" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N77)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F77" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N77)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G77" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N77)&gt;=70,IF((N77-50)&gt;50,50,IF((N77-50)&lt;0,0,(N77-50))), "" )</f>
         <v>31</v>
       </c>
       <c r="H77">
@@ -4672,7 +4708,7 @@
         <v>25</v>
       </c>
       <c r="N77">
-        <f t="shared" si="9"/>
+        <f>IF((H77+I77+J77+L77+M77+O77)&lt;70,IF((H77+I77+J77+L77+M77+O77)&gt;59,70,(H77+I77+J77+L77+M77+O77)),(H77+I77+J77+L77+M77+O77))</f>
         <v>81</v>
       </c>
     </row>
@@ -4686,21 +4722,21 @@
       <c r="C78" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D78" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E78" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G78" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D78" s="6">
+        <f>IF((N78)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E78" s="2">
+        <f>IF((N78)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F78" s="2">
+        <f>IF((N78)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G78" s="6">
+        <f>IF((N78)&gt;=70,IF((N78-50)&gt;50,50,IF((N78-50)&lt;0,0,(N78-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H78">
         <v>14</v>
@@ -4714,9 +4750,12 @@
       <c r="K78">
         <v>1</v>
       </c>
+      <c r="M78">
+        <v>28</v>
+      </c>
       <c r="N78">
-        <f t="shared" si="9"/>
-        <v>36</v>
+        <f>IF((H78+I78+J78+L78+M78+O78)&lt;70,IF((H78+I78+J78+L78+M78+O78)&gt;59,70,(H78+I78+J78+L78+M78+O78)),(H78+I78+J78+L78+M78+O78))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4729,21 +4768,21 @@
       <c r="C79" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D79" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E79" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G79" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D79" s="6">
+        <f>IF((N79)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E79" s="2">
+        <f>IF((N79)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F79" s="2">
+        <f>IF((N79)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G79" s="6">
+        <f>IF((N79)&gt;=70,IF((N79-50)&gt;50,50,IF((N79-50)&lt;0,0,(N79-50))), "" )</f>
+        <v>37</v>
       </c>
       <c r="H79">
         <v>14</v>
@@ -4760,9 +4799,12 @@
       <c r="L79">
         <v>20</v>
       </c>
+      <c r="M79">
+        <v>28</v>
+      </c>
       <c r="N79">
-        <f t="shared" si="9"/>
-        <v>59</v>
+        <f>IF((H79+I79+J79+L79+M79+O79)&lt;70,IF((H79+I79+J79+L79+M79+O79)&gt;59,70,(H79+I79+J79+L79+M79+O79)),(H79+I79+J79+L79+M79+O79))</f>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4775,21 +4817,21 @@
       <c r="C80" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="D80" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E80" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G80" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D80" s="6">
+        <f>IF((N80)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E80" s="2">
+        <f>IF((N80)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F80" s="2">
+        <f>IF((N80)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G80" s="6">
+        <f>IF((N80)&gt;=70,IF((N80-50)&gt;50,50,IF((N80-50)&lt;0,0,(N80-50))), "" )</f>
+        <v>33</v>
       </c>
       <c r="H80">
         <v>16</v>
@@ -4806,9 +4848,12 @@
       <c r="L80">
         <v>15</v>
       </c>
+      <c r="M80">
+        <v>30</v>
+      </c>
       <c r="N80">
-        <f t="shared" si="9"/>
-        <v>53</v>
+        <f>IF((H80+I80+J80+L80+M80+O80)&lt;70,IF((H80+I80+J80+L80+M80+O80)&gt;59,70,(H80+I80+J80+L80+M80+O80)),(H80+I80+J80+L80+M80+O80))</f>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4822,20 +4867,20 @@
         <v>173</v>
       </c>
       <c r="D81" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N81)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N81)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F81" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N81)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G81" s="6">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <f>IF((N81)&gt;=70,IF((N81-50)&gt;50,50,IF((N81-50)&lt;0,0,(N81-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H81">
         <v>18</v>
@@ -4852,9 +4897,12 @@
       <c r="L81">
         <v>20</v>
       </c>
+      <c r="M81">
+        <v>30</v>
+      </c>
       <c r="N81">
-        <f t="shared" si="9"/>
-        <v>70</v>
+        <f>IF((H81+I81+J81+L81+M81+O81)&lt;70,IF((H81+I81+J81+L81+M81+O81)&gt;59,70,(H81+I81+J81+L81+M81+O81)),(H81+I81+J81+L81+M81+O81))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4868,19 +4916,19 @@
         <v>175</v>
       </c>
       <c r="D82" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N82)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N82)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F82" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N82)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G82" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N82)&gt;=70,IF((N82-50)&gt;50,50,IF((N82-50)&lt;0,0,(N82-50))), "" )</f>
         <v>33</v>
       </c>
       <c r="H82">
@@ -4902,7 +4950,7 @@
         <v>29</v>
       </c>
       <c r="N82">
-        <f t="shared" si="9"/>
+        <f>IF((H82+I82+J82+L82+M82+O82)&lt;70,IF((H82+I82+J82+L82+M82+O82)&gt;59,70,(H82+I82+J82+L82+M82+O82)),(H82+I82+J82+L82+M82+O82))</f>
         <v>83</v>
       </c>
     </row>
@@ -4917,20 +4965,20 @@
         <v>177</v>
       </c>
       <c r="D83" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N83)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E83" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N83)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F83" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N83)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G83" s="6">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <f>IF((N83)&gt;=70,IF((N83-50)&gt;50,50,IF((N83-50)&lt;0,0,(N83-50))), "" )</f>
+        <v>48</v>
       </c>
       <c r="H83">
         <v>23</v>
@@ -4947,9 +4995,12 @@
       <c r="L83">
         <v>15</v>
       </c>
+      <c r="M83">
+        <v>30</v>
+      </c>
       <c r="N83">
-        <f t="shared" si="9"/>
-        <v>70</v>
+        <f>IF((H83+I83+J83+L83+M83+O83)&lt;70,IF((H83+I83+J83+L83+M83+O83)&gt;59,70,(H83+I83+J83+L83+M83+O83)),(H83+I83+J83+L83+M83+O83))</f>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4963,19 +5014,19 @@
         <v>179</v>
       </c>
       <c r="D84" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N84)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E84" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N84)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F84" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N84)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G84" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N84)&gt;=70,IF((N84-50)&gt;50,50,IF((N84-50)&lt;0,0,(N84-50))), "" )</f>
         <v>50</v>
       </c>
       <c r="H84">
@@ -4997,7 +5048,7 @@
         <v>29</v>
       </c>
       <c r="N84">
-        <f t="shared" si="9"/>
+        <f>IF((H84+I84+J84+L84+M84+O84)&lt;70,IF((H84+I84+J84+L84+M84+O84)&gt;59,70,(H84+I84+J84+L84+M84+O84)),(H84+I84+J84+L84+M84+O84))</f>
         <v>102</v>
       </c>
     </row>
@@ -5012,20 +5063,20 @@
         <v>181</v>
       </c>
       <c r="D85" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N85)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E85" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N85)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F85" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N85)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G85" s="6">
-        <f t="shared" si="8"/>
-        <v>23</v>
+        <f>IF((N85)&gt;=70,IF((N85-50)&gt;50,50,IF((N85-50)&lt;0,0,(N85-50))), "" )</f>
+        <v>38</v>
       </c>
       <c r="H85">
         <v>17</v>
@@ -5043,11 +5094,11 @@
         <v>15</v>
       </c>
       <c r="M85">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="N85">
-        <f t="shared" si="9"/>
-        <v>73</v>
+        <f>IF((H85+I85+J85+L85+M85+O85)&lt;70,IF((H85+I85+J85+L85+M85+O85)&gt;59,70,(H85+I85+J85+L85+M85+O85)),(H85+I85+J85+L85+M85+O85))</f>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5061,19 +5112,19 @@
         <v>183</v>
       </c>
       <c r="D86" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N86)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N86)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F86" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N86)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N86)&gt;=70,IF((N86-50)&gt;50,50,IF((N86-50)&lt;0,0,(N86-50))), "" )</f>
         <v>40</v>
       </c>
       <c r="H86">
@@ -5095,7 +5146,7 @@
         <v>30</v>
       </c>
       <c r="N86">
-        <f t="shared" si="9"/>
+        <f>IF((H86+I86+J86+L86+M86+O86)&lt;70,IF((H86+I86+J86+L86+M86+O86)&gt;59,70,(H86+I86+J86+L86+M86+O86)),(H86+I86+J86+L86+M86+O86))</f>
         <v>90</v>
       </c>
     </row>
@@ -5110,20 +5161,20 @@
         <v>185</v>
       </c>
       <c r="D87" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N87)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N87)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F87" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N87)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G87" s="6">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <f>IF((N87)&gt;=70,IF((N87-50)&gt;50,50,IF((N87-50)&lt;0,0,(N87-50))), "" )</f>
+        <v>48</v>
       </c>
       <c r="H87">
         <v>23</v>
@@ -5140,9 +5191,12 @@
       <c r="L87">
         <v>15</v>
       </c>
+      <c r="M87">
+        <v>30</v>
+      </c>
       <c r="N87">
-        <f t="shared" si="9"/>
-        <v>70</v>
+        <f>IF((H87+I87+J87+L87+M87+O87)&lt;70,IF((H87+I87+J87+L87+M87+O87)&gt;59,70,(H87+I87+J87+L87+M87+O87)),(H87+I87+J87+L87+M87+O87))</f>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5156,19 +5210,19 @@
         <v>187</v>
       </c>
       <c r="D88" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N88)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E88" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N88)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F88" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N88)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G88" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N88)&gt;=70,IF((N88-50)&gt;50,50,IF((N88-50)&lt;0,0,(N88-50))), "" )</f>
         <v>33</v>
       </c>
       <c r="H88">
@@ -5190,7 +5244,7 @@
         <v>25</v>
       </c>
       <c r="N88">
-        <f t="shared" si="9"/>
+        <f>IF((H88+I88+J88+L88+M88+O88)&lt;70,IF((H88+I88+J88+L88+M88+O88)&gt;59,70,(H88+I88+J88+L88+M88+O88)),(H88+I88+J88+L88+M88+O88))</f>
         <v>83</v>
       </c>
     </row>
@@ -5205,19 +5259,19 @@
         <v>189</v>
       </c>
       <c r="D89" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N89)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E89" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N89)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F89" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N89)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G89" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N89)&gt;=70,IF((N89-50)&gt;50,50,IF((N89-50)&lt;0,0,(N89-50))), "" )</f>
         <v>36</v>
       </c>
       <c r="H89">
@@ -5239,7 +5293,7 @@
         <v>30</v>
       </c>
       <c r="N89">
-        <f t="shared" si="9"/>
+        <f>IF((H89+I89+J89+L89+M89+O89)&lt;70,IF((H89+I89+J89+L89+M89+O89)&gt;59,70,(H89+I89+J89+L89+M89+O89)),(H89+I89+J89+L89+M89+O89))</f>
         <v>86</v>
       </c>
     </row>
@@ -5253,21 +5307,21 @@
       <c r="C90" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D90" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E90" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F90" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G90" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D90" s="6">
+        <f>IF((N90)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E90" s="2">
+        <f>IF((N90)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F90" s="2">
+        <f>IF((N90)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G90" s="6">
+        <f>IF((N90)&gt;=70,IF((N90-50)&gt;50,50,IF((N90-50)&lt;0,0,(N90-50))), "" )</f>
+        <v>21</v>
       </c>
       <c r="I90">
         <v>10</v>
@@ -5281,9 +5335,12 @@
       <c r="L90">
         <v>20</v>
       </c>
+      <c r="M90">
+        <v>28</v>
+      </c>
       <c r="N90">
-        <f t="shared" si="9"/>
-        <v>43</v>
+        <f>IF((H90+I90+J90+L90+M90+O90)&lt;70,IF((H90+I90+J90+L90+M90+O90)&gt;59,70,(H90+I90+J90+L90+M90+O90)),(H90+I90+J90+L90+M90+O90))</f>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5297,19 +5354,19 @@
         <v>193</v>
       </c>
       <c r="D91" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N91)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E91" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N91)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F91" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N91)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G91" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N91)&gt;=70,IF((N91-50)&gt;50,50,IF((N91-50)&lt;0,0,(N91-50))), "" )</f>
         <v/>
       </c>
       <c r="H91">
@@ -5328,7 +5385,7 @@
         <v>15</v>
       </c>
       <c r="N91">
-        <f t="shared" si="9"/>
+        <f>IF((H91+I91+J91+L91+M91+O91)&lt;70,IF((H91+I91+J91+L91+M91+O91)&gt;59,70,(H91+I91+J91+L91+M91+O91)),(H91+I91+J91+L91+M91+O91))</f>
         <v>52</v>
       </c>
     </row>
@@ -5343,19 +5400,19 @@
         <v>195</v>
       </c>
       <c r="D92" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N92)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E92" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N92)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F92" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N92)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G92" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N92)&gt;=70,IF((N92-50)&gt;50,50,IF((N92-50)&lt;0,0,(N92-50))), "" )</f>
         <v/>
       </c>
       <c r="H92">
@@ -5374,7 +5431,7 @@
         <v>15</v>
       </c>
       <c r="N92">
-        <f t="shared" si="9"/>
+        <f>IF((H92+I92+J92+L92+M92+O92)&lt;70,IF((H92+I92+J92+L92+M92+O92)&gt;59,70,(H92+I92+J92+L92+M92+O92)),(H92+I92+J92+L92+M92+O92))</f>
         <v>54</v>
       </c>
     </row>
@@ -5389,19 +5446,19 @@
         <v>197</v>
       </c>
       <c r="D93" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N93)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E93" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N93)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F93" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N93)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G93" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N93)&gt;=70,IF((N93-50)&gt;50,50,IF((N93-50)&lt;0,0,(N93-50))), "" )</f>
         <v>32</v>
       </c>
       <c r="H93">
@@ -5423,7 +5480,7 @@
         <v>28</v>
       </c>
       <c r="N93">
-        <f t="shared" si="9"/>
+        <f>IF((H93+I93+J93+L93+M93+O93)&lt;70,IF((H93+I93+J93+L93+M93+O93)&gt;59,70,(H93+I93+J93+L93+M93+O93)),(H93+I93+J93+L93+M93+O93))</f>
         <v>82</v>
       </c>
     </row>
@@ -5437,21 +5494,21 @@
       <c r="C94" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D94" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E94" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F94" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G94" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D94" s="6">
+        <f>IF((N94)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E94" s="2">
+        <f>IF((N94)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F94" s="2">
+        <f>IF((N94)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G94" s="6">
+        <f>IF((N94)&gt;=70,IF((N94-50)&gt;50,50,IF((N94-50)&lt;0,0,(N94-50))), "" )</f>
+        <v>30</v>
       </c>
       <c r="H94">
         <v>15</v>
@@ -5468,9 +5525,12 @@
       <c r="L94">
         <v>20</v>
       </c>
+      <c r="M94">
+        <v>23</v>
+      </c>
       <c r="N94">
-        <f t="shared" si="9"/>
-        <v>57</v>
+        <f>IF((H94+I94+J94+L94+M94+O94)&lt;70,IF((H94+I94+J94+L94+M94+O94)&gt;59,70,(H94+I94+J94+L94+M94+O94)),(H94+I94+J94+L94+M94+O94))</f>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5484,30 +5544,27 @@
         <v>201</v>
       </c>
       <c r="D95" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N95)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E95" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N95)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F95" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N95)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G95" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I95">
-        <v>10</v>
+        <f>IF((N95)&gt;=70,IF((N95-50)&gt;50,50,IF((N95-50)&lt;0,0,(N95-50))), "" )</f>
+        <v/>
       </c>
       <c r="K95">
         <v>1</v>
       </c>
       <c r="N95">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f>IF((H95+I95+J95+L95+M95+O95)&lt;70,IF((H95+I95+J95+L95+M95+O95)&gt;59,70,(H95+I95+J95+L95+M95+O95)),(H95+I95+J95+L95+M95+O95))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5521,19 +5578,19 @@
         <v>203</v>
       </c>
       <c r="D96" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N96)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E96" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N96)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F96" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N96)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G96" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N96)&gt;=70,IF((N96-50)&gt;50,50,IF((N96-50)&lt;0,0,(N96-50))), "" )</f>
         <v/>
       </c>
       <c r="I96">
@@ -5549,7 +5606,7 @@
         <v>20</v>
       </c>
       <c r="N96">
-        <f t="shared" si="9"/>
+        <f>IF((H96+I96+J96+L96+M96+O96)&lt;70,IF((H96+I96+J96+L96+M96+O96)&gt;59,70,(H96+I96+J96+L96+M96+O96)),(H96+I96+J96+L96+M96+O96))</f>
         <v>36</v>
       </c>
     </row>
@@ -5564,19 +5621,19 @@
         <v>205</v>
       </c>
       <c r="D97" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N97)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E97" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N97)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F97" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N97)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G97" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N97)&gt;=70,IF((N97-50)&gt;50,50,IF((N97-50)&lt;0,0,(N97-50))), "" )</f>
         <v/>
       </c>
       <c r="H97">
@@ -5592,7 +5649,7 @@
         <v>1</v>
       </c>
       <c r="N97">
-        <f t="shared" si="9"/>
+        <f>IF((H97+I97+J97+L97+M97+O97)&lt;70,IF((H97+I97+J97+L97+M97+O97)&gt;59,70,(H97+I97+J97+L97+M97+O97)),(H97+I97+J97+L97+M97+O97))</f>
         <v>35</v>
       </c>
     </row>
@@ -5607,19 +5664,19 @@
         <v>207</v>
       </c>
       <c r="D98" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N98)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E98" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N98)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F98" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N98)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G98" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N98)&gt;=70,IF((N98-50)&gt;50,50,IF((N98-50)&lt;0,0,(N98-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H98">
@@ -5641,7 +5698,7 @@
         <v>15</v>
       </c>
       <c r="N98">
-        <f t="shared" si="9"/>
+        <f>IF((H98+I98+J98+L98+M98+O98)&lt;70,IF((H98+I98+J98+L98+M98+O98)&gt;59,70,(H98+I98+J98+L98+M98+O98)),(H98+I98+J98+L98+M98+O98))</f>
         <v>70</v>
       </c>
     </row>
@@ -5650,30 +5707,27 @@
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
       <c r="D99" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N99)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E99" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N99)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F99" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N99)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G99" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I99">
-        <v>10</v>
+        <f>IF((N99)&gt;=70,IF((N99-50)&gt;50,50,IF((N99-50)&lt;0,0,(N99-50))), "" )</f>
+        <v/>
       </c>
       <c r="K99">
         <v>1</v>
       </c>
       <c r="N99">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f>IF((H99+I99+J99+L99+M99+O99)&lt;70,IF((H99+I99+J99+L99+M99+O99)&gt;59,70,(H99+I99+J99+L99+M99+O99)),(H99+I99+J99+L99+M99+O99))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5698,11 +5752,14 @@
     <row r="119" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="120" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:O1">
+  <autoFilter ref="A1:O99">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="6" showButton="0"/>
+    <sortState ref="A2:O99">
+      <sortCondition ref="A1:A99"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.39" right="0.39" top="0.39" bottom="0.39" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>